<commit_message>
Cambios documentacion y modelos BD
</commit_message>
<xml_diff>
--- a/ARCHIVOS/Historias de usuario.xlsx
+++ b/ARCHIVOS/Historias de usuario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yesenia\Documents\YESENIA\CLASES DEL SENA\Proyecto__SENA\ARCHIVOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A108C6-0857-4FE0-8A7F-1E6863FD224E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55152925-40EE-4BD3-BA89-74062F2D4703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,12 +144,6 @@
  PARA visualizar los servicios publicados desde el más reciente hasta el más antiguo </t>
   </si>
   <si>
-    <t>Se debe crear una pagina principal en la cual el perfil de cliente va a poder visualizar todos los servicios publicados de los mas recientes a los mas antiguos, mostrara la imagen, el titulo de la publicación y tendra un boton de mas informacion que pasara a mostrar todos los datos del producto individual, en la pagina principal tendra las opciones de menu, busquedad, inicio, perfil y categorias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) Se debe realizar una página principal donde se puedan visualizar los productos del más reciente al más antiguo.  2) Se debe realizar una tarjeta por cada servicio publicado con su respectiva imagen y titulo, tendra un boton de más información que lo llevará directamente a la informacion completa tanto del producto como del proveedor. 3) Se debe realizar un barra de navegación superior que contenga los iconos de menu, el logo y la opcion de busquedad. 4) Se debe realizar una barra de navegación inferior que contenga los iconos inicio, perfil y categorías </t>
-  </si>
-  <si>
     <t>COMO cliente
  QUIERO que haya un icono 
  PARA visualizar las categorias de los servicios publicados</t>
@@ -188,6 +182,14 @@
   </si>
   <si>
     <t>Se debe crear un registro que le permita al usuario ingresar los siguientes datos para contar con un perfil en el aplicativo, N° de identificacion, fecha de nacimiento nombres, apellidos, direccion, celular, correo electronico, contraseña nueva y escoger el perfil de entrada de su preferencia.</t>
+  </si>
+  <si>
+    <t>Se debe crear una página principal en la cual el perfil de cliente va a poder visualizar todos los servicios publicados de los más recientes a los más antiguos, mostrara la imagen, el título de la publicación, y una breve descripción de los términos y tendrá un botón de más información que lo llevara a otra página que mostrara todos los datos del producto de manera más específica, en la página principal tendrá una barra de navegación con diferentes funcionalidades.</t>
+  </si>
+  <si>
+    <t>1) Se debe realizar una página principal donde se puedan visualizar los productos del más reciente al más antiguo. 
+ 2) Se debe realizar una tarjeta por cada servicio publicado con su respectiva imagen, nombre, precio, y una breve descripción de los términos, también tendrá un botón de más información que lo llevará directamente a la información completa tanto del producto como del proveedor que realizo la publicación. 
+3) Se debe realizar una barra de navegación donde podrá visualizar con mayor facilidad las funcionalidades de acuerdo con su perfil como cliente.</t>
   </si>
 </sst>
 </file>
@@ -568,8 +570,8 @@
   </sheetPr>
   <dimension ref="A1:E994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -609,10 +611,10 @@
         <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -620,7 +622,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>26</v>
@@ -654,7 +656,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>29</v>
@@ -671,7 +673,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>14</v>
@@ -688,16 +690,16 @@
         <v>15</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="E7" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="122.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -705,7 +707,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>34</v>
@@ -714,7 +716,7 @@
         <v>35</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="150.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -728,7 +730,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>36</v>

</xml_diff>